<commit_message>
Create button to run without showing faces
</commit_message>
<xml_diff>
--- a/src/Results/Results.xlsx
+++ b/src/Results/Results.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>neutral</t>
   </si>
   <si>
-    <t>angry</t>
+    <t>fear</t>
+  </si>
+  <si>
+    <t>surprise</t>
   </si>
   <si>
     <t>happy</t>
@@ -380,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -413,7 +416,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>8.384979099995689</v>
+        <v>1.02808640000876</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -424,7 +427,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>8.608741099989857</v>
+        <v>1.24741820001509</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -435,7 +438,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>9.758527400001185</v>
+        <v>2.994884000014281</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -446,7 +449,40 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>10.9394384999905</v>
+        <v>3.202956299996004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3.436031999997795</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>4.098535500001162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4.34527469999739</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start and stop analysis button working
</commit_message>
<xml_diff>
--- a/src/Results/Results.xlsx
+++ b/src/Results/Results.xlsx
@@ -14,18 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
   <si>
     <t>neutral</t>
+  </si>
+  <si>
+    <t>sad</t>
   </si>
   <si>
     <t>fear</t>
   </si>
   <si>
-    <t>surprise</t>
+    <t>happy</t>
   </si>
   <si>
-    <t>happy</t>
+    <t>angry</t>
+  </si>
+  <si>
+    <t>surprise</t>
   </si>
 </sst>
 </file>
@@ -383,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -416,7 +422,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.02808640000876</v>
+        <v>1.062102600000799</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -424,10 +430,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>1.24741820001509</v>
+        <v>1.463099300002796</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -435,10 +441,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>2.994884000014281</v>
+        <v>1.678607100009685</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -446,10 +452,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>3.202956299996004</v>
+        <v>2.135661699998309</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -457,10 +463,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>3.436031999997795</v>
+        <v>2.712933200004045</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -468,10 +474,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>4.098535500001162</v>
+        <v>2.911483200005023</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -479,10 +485,153 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>4.82185040001059</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C9">
-        <v>4.34527469999739</v>
+      <c r="C10">
+        <v>5.059743100006017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>5.875170300001628</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>6.073256500007119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>6.470396800010349</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>7.110622200008947</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>7.498422500008019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>8.126322500000242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>13.64557620001142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>18.32348210000782</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>18.54596410000522</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>18.74780310000642</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>19.64774410000246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>20.6621487000084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All buttons working properly
</commit_message>
<xml_diff>
--- a/src/Results/Results.xlsx
+++ b/src/Results/Results.xlsx
@@ -14,24 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>neutral</t>
   </si>
   <si>
-    <t>sad</t>
-  </si>
-  <si>
-    <t>fear</t>
-  </si>
-  <si>
     <t>happy</t>
-  </si>
-  <si>
-    <t>angry</t>
-  </si>
-  <si>
-    <t>surprise</t>
   </si>
 </sst>
 </file>
@@ -389,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -422,216 +410,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.062102600000799</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1.463099300002796</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1.678607100009685</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>2.135661699998309</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>2.712933200004045</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>2.911483200005023</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>4.82185040001059</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>5.059743100006017</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>5.875170300001628</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>6.073256500007119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>6.470396800010349</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>7.110622200008947</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>7.498422500008019</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>8.126322500000242</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>13.64557620001142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>18.32348210000782</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>18.54596410000522</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <v>18.74780310000642</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>19.64774410000246</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>20.6621487000084</v>
+        <v>1.558637000001909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>